<commit_message>
Plugin de push añadido de nuevo
</commit_message>
<xml_diff>
--- a/Assets/Localization/2017 YB QuotesLocalization_xls_modif.xlsx
+++ b/Assets/Localization/2017 YB QuotesLocalization_xls_modif.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity\Nemoris\FraseDiaria\Assets\Localization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NemorisGames\NemorisGamesUnity\FraseDiaria\FraseDiaria\Assets\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2247,92 +2247,89 @@
     <t>Lenguaje</t>
   </si>
   <si>
-    <t>NOTE: The quotes in this calendar have been edited. 
- These quotes have been altered by the editors for 
-proper grammar and understanding while ensuring 
-that the core message has been preserved.
+    <t>HISTORY LABEL</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>NOTE: The quotes in this calendar have been edited. These quotes have been altered by the editors for proper grammar and understanding while ensuring that the core message has been preserved.
 Copyright © 2016 Aquarian Wisdom. All teachings, yoga sets, techniques, kriyas and meditations courtesy of The Teachings of Yogi Bhajan. Reprinted with permission. Unauthorized duplication is a violation of applicable laws. ALL RIGHTS RESERVED. No part of these Teachings may be reproduced or transmitted in any form by any means, electronic or mechanical, including photocopying and recording, or by any information storage and retrieval system, except as may be expressly permitted in writing by the The Teachings of Yogi Bhajan. To request permission, please write to KRI at PO Box 1819, Santa Cruz, NM 87567 or see Kundalini Research Institute – Kundalini Yoga As Taught By Yogi Bhajan</t>
-  </si>
-  <si>
-    <t>HISTORY LABEL</t>
-  </si>
-  <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
-    <t>Enero</t>
-  </si>
-  <si>
-    <t>Febrero</t>
-  </si>
-  <si>
-    <t>Marzo</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t>Mayo</t>
-  </si>
-  <si>
-    <t>Junio</t>
-  </si>
-  <si>
-    <t>Julio</t>
-  </si>
-  <si>
-    <t>Agosto</t>
-  </si>
-  <si>
-    <t>Octubre</t>
-  </si>
-  <si>
-    <t>Noviembre</t>
-  </si>
-  <si>
-    <t>Diciembre</t>
-  </si>
-  <si>
-    <t>Septiembre</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Mes</t>
   </si>
 </sst>
 </file>
@@ -2880,7 +2877,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2923,6 +2920,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3247,7 +3247,7 @@
   <dimension ref="A1:F384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,9 +3285,9 @@
         <v>738</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>742</v>
-      </c>
-      <c r="E2" s="8"/>
+        <v>769</v>
+      </c>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -3360,223 +3360,223 @@
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>767</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>768</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>743</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>768</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>743</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>744</v>
-      </c>
       <c r="E8" s="9" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>